<commit_message>
Accept project path as argument and change the column Severity to Action.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DC2AB3-FFD6-4108-80F0-5C1E13823A9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E501BDB2-1835-4607-89A3-06708C76619C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -218,64 +218,60 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Medium</t>
+    <t>Checks\UndocumentedDefaultClick.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Use SimulateClick or SendWindowMessages if the target control supports it.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Since they do not depend on the mouse driver, the properties SimulateClick and SendWindowMessages provide a faster and more robust way to perform clicks, so they should be used whenever possible. Alternatively, add an annotation in case the control does not support such properties. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Since they do not depend on the keyboard driver, the properties SimulateType and SendWindowMessages provide a faster and more robust way to perform typing actions, so they should be used whenever possible. Alternatively, add an annotation in case the control does not support such properties. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Use SimulateType or SendWindowMessages if the target control supports it.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\UndocumentedDefaultType.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Undocumented default type</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Undocumented default click</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Undocumented unreachable activities</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\UndocumentedUnreachableActivities.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>If no action is taken to handle the exception, consider including at least a Log Message activity and Rethrow it.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Action</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>High</t>
+    <t>Fix</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Severity</t>
+    <t>Double check</t>
     <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Low</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDefaultClick.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use SimulateClick or SendWindowMessages if the target control supports it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Since they do not depend on the mouse driver, the properties SimulateClick and SendWindowMessages provide a faster and more robust way to perform clicks, so they should be used whenever possible. Alternatively, add an annotation in case the control does not support such properties. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Since they do not depend on the keyboard driver, the properties SimulateType and SendWindowMessages provide a faster and more robust way to perform typing actions, so they should be used whenever possible. Alternatively, add an annotation in case the control does not support such properties. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use SimulateType or SendWindowMessages if the target control supports it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDefaultType.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Undocumented default type</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Undocumented default click</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Undocumented unreachable activities</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UndocumentedUnreachableActivities.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>If no action is taken to handle the exception, consider including at least a Log Message activity and Rethrow it.</t>
-    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -1609,7 +1605,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
@@ -1637,7 +1633,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1658,7 +1654,7 @@
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
@@ -1679,7 +1675,7 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
@@ -1700,7 +1696,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>15</v>
@@ -1721,13 +1717,13 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1744,7 +1740,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>23</v>
@@ -1767,7 +1763,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>28</v>
@@ -1781,20 +1777,20 @@
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1802,20 +1798,20 @@
         <v>1</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
@@ -1832,7 +1828,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>30</v>
@@ -1853,7 +1849,7 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>41</v>
@@ -1867,14 +1863,14 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>45</v>
@@ -2172,7 +2168,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -2193,7 +2189,7 @@
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Made it possible to select different features to be executed.
Currently only Check Best Practices implemented.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E501BDB2-1835-4607-89A3-06708C76619C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA82ED0-0BEA-4AD3-BC82-801CE935AD48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -51,18 +51,10 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\MissingWorkflowAnnotation.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Missing screenshot</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\MissingScreenshot.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Other than textual descriptions, screenshots are helpful in explaining what the activity does and with what elements it interacts. The screenshots should be stored in the .screenshots folder of the project.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -87,27 +79,15 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\UndocumentedDelay.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Empty Catch block</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\EmptyCatchBlock.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Exceptions should be caught with a purpose, not only to prevent error messages. For this reason, it is recommended to insert log messages in the Catch block of a Try Catch activity, in addition to the exception handling itself. For more about error handling, refer to https://studio.uipath.com/docs/project-organization#section-error-handling</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Variables not following naming convention</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\VariableNamingConvention.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -131,10 +111,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\ArgumentNamingConvention.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Arguments in a project should follow a specified naming convention, since it makes it easier to understand the project and maintain it. This check receives a regular expression that dictates the naming convention for arguments. For more information about naming conventions, refer to https://studio.uipath.com/docs/workflow-design#section-naming-conventions</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -155,19 +131,11 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\LargeIdxInSelector.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>The project.json file contains important information about the project and it is used by UiPath Studio when loading the project. For more information about this file, refer to https://studio.uipath.com/docs/about-the-projectjson-file</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Create or import a project.json file for the project.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\ProjectJsonConfigurationFile.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -194,10 +162,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\UnnecessarySequenceOrFlowchart.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Remove sequences or flowcharts that are empty or contain only one activity.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -210,18 +174,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Severity</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Low</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDefaultClick.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Use SimulateClick or SendWindowMessages if the target control supports it.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -238,10 +190,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\UndocumentedDefaultType.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Undocumented default type</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -251,10 +199,6 @@
   </si>
   <si>
     <t>Undocumented unreachable activities</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UndocumentedUnreachableActivities.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -272,6 +216,54 @@
   <si>
     <t>Double check</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\MissingWorkflowAnnotation.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\MissingScreenshot.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\UndocumentedDelay.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\EmptyCatchBlock.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\VariableNamingConvention.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\ArgumentNamingConvention.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\UndocumentedDefaultClick.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\UndocumentedDefaultType.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\LargeIdxInSelector.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\UnnecessarySequenceOrFlowchart.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\UndocumentedUnreachableActivities.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>CheckBestPractices\Checks\ProjectJsonConfigurationFile.xaml</t>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -1605,7 +1597,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
@@ -1621,7 +1613,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>4</v>
@@ -1633,7 +1625,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1650,17 +1642,17 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
@@ -1668,20 +1660,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
@@ -1689,20 +1681,20 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
@@ -1710,20 +1702,20 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1731,22 +1723,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1754,22 +1746,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1777,20 +1769,20 @@
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1798,20 +1790,20 @@
         <v>1</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
@@ -1819,22 +1811,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="187.5">
@@ -1842,20 +1834,20 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="93.75">
@@ -1863,20 +1855,20 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +2133,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2156,10 +2148,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -2168,7 +2160,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -2182,20 +2174,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed parts related to workflow statistics.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE3CC79-CAC6-4CD3-84B3-D753C0CA4684}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD10AFAA-457A-456F-82CC-A2BEC0C3E0D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -1588,9 +1588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -1854,7 +1852,7 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>36</v>
@@ -2124,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
Setting check for minimum scope not to run as default.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBA8786-623D-491C-9282-FCED9C0A4F13}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148BA87C-0948-474F-A350-E5A07D0547A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -315,6 +315,9 @@
   <si>
     <t>Define unique names for variables and arguments.</t>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{FACCEB44-97B3-401B-BD48-08626DAD862C}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -760,15 +763,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="28.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="1"/>
+    <col min="1" max="1" width="8.58203125" style="1"/>
+    <col min="2" max="2" width="15.58203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="28.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.58203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -794,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>
@@ -815,7 +818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="72">
       <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
@@ -836,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
@@ -857,7 +860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="126">
       <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
@@ -878,7 +881,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A6" s="9" t="s">
         <v>62</v>
       </c>
@@ -901,7 +904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A7" s="9" t="s">
         <v>62</v>
       </c>
@@ -924,7 +927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A8" s="9" t="s">
         <v>62</v>
       </c>
@@ -945,7 +948,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A9" s="9" t="s">
         <v>62</v>
       </c>
@@ -966,7 +969,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="162">
       <c r="A10" s="9" t="s">
         <v>62</v>
       </c>
@@ -989,7 +992,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="187.5">
+    <row r="11" spans="1:7" ht="180">
       <c r="A11" s="9" t="s">
         <v>62</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="93.75">
+    <row r="12" spans="1:7" ht="90">
       <c r="A12" s="9" t="s">
         <v>62</v>
       </c>
@@ -1031,9 +1034,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="56.25">
+    <row r="13" spans="1:7" ht="54">
       <c r="A13" s="9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>63</v>
@@ -1052,7 +1055,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75">
+    <row r="14" spans="1:7" ht="54">
       <c r="A14" s="9" t="s">
         <v>68</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="75">
+    <row r="15" spans="1:7" ht="72">
       <c r="A15" s="9" t="s">
         <v>68</v>
       </c>
@@ -1097,7 +1100,7 @@
   </sheetData>
   <phoneticPr fontId="6"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A12 A14:A15" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1114,14 +1117,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="5" width="28.375" customWidth="1"/>
-    <col min="6" max="6" width="49.875" customWidth="1"/>
-    <col min="7" max="7" width="40.125" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="49.83203125" customWidth="1"/>
+    <col min="7" max="7" width="40.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1147,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Added the description of remaining checks to be implemented.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148BA87C-0948-474F-A350-E5A07D0547A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD446940-8B3A-4025-8F40-ABB2C3CCD1F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="100">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -266,58 +266,144 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
+    <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Restrict the scope of the variable.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\VariableMinimumScope\VariableMinimumScope.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Variable overrides variable</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\VariableOverridesVariable.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Although it is technically possible for two variables to have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Define unique names for variables, even if they are in different scopes.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Variable overrides argument</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\VariableOverridesArgument.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Although it is technically possible for a variable and an argument have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Define unique names for variables and arguments.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Fix</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Restrict the scope of the variable.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\VariableMinimumScope\VariableMinimumScope.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Variable overrides variable</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\VariableOverridesVariable.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Although it is technically possible for two variables to have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Define unique names for variables, even if they are in different scopes.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variable overrides argument</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\VariableOverridesArgument.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Although it is technically possible for a variable and an argument have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Define unique names for variables and arguments.</t>
+  </si>
+  <si>
+    <t>Double check</t>
+  </si>
+  <si>
+    <t>Deeply nested activities</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\DeeplyNestedActivities.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>It is usually more difficult to see and understand workflows that have too many deeply nested activities, so it is recommended to avoid deeply nested structures. Instead, it might be better to separate the workflow into smaller ones and use the Invoke Workflow File activity to call them.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Consider dividing the workflow into smaller components to avoid deeply nested structures.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Unused variables</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\UnusedVariables.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Workflows should only have variables and arguments that are necessary for its execution. Unused variables and arguments make the project more difficult to understand and should be removed. For removing all unsed variables, use the button "Remove Unused Variables" in UiPath Studio (https://studio.uipath.com/docs/managing-variables#section-removing-variables)</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Remove variables and arguments that are not being used.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\OpenApplicationBrowser.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Open Browser not being used</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>The Open Browser activity provides a convenient way to open a browser tab or window, and it also serves as a container for activities related to web automation. For this reason, it should be the preferred way to work with browsers, instead of Open Application or Start Process.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Consider the use of Open Browser instead of Open Application or Start Process.</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>No</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Hotkey without selector</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\HotkeyWithoutSelector.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Send Hotkey activities without selector can be intercepted by any application that comes to the foreground (for example, Windows notifications and antivirus popups), which will prevent the intended execution. For this reason, it is recommended to use selectors or include them in containers that have selectors (for example, Attach Window or Attach Browser).</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Specify a selector when using Send Hotkey activity or include it inside a container.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Repeated display names for activities</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\RepeatedActivitiyName.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>The names of the activities should give a clear idea of how it is being used. Although the default names usually provide a good description, sometimes they are too generic, so it is recommended to add more information when the context is not clear. This check looks for activities that have the same name, which might indicate that the same generic name is used multiple times. The check accepts an argument which is the threshold of how many activities can have the same name.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Check if it could be easier to understand what the activity does by adding a more descriptive title.</t>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -759,9 +845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18"/>
   <cols>
@@ -939,7 +1027,7 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>39</v>
@@ -960,7 +1048,7 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>40</v>
@@ -983,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>24</v>
@@ -1004,7 +1092,7 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>33</v>
@@ -1025,7 +1113,7 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>36</v>
@@ -1036,72 +1124,203 @@
     </row>
     <row r="13" spans="1:7" ht="54">
       <c r="A13" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="54">
       <c r="A14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="72">
       <c r="A15" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="4" t="s">
+    </row>
+    <row r="16" spans="1:7" ht="108">
+      <c r="A16" s="9" t="s">
         <v>76</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="6">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="126">
+      <c r="A17" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="90">
+      <c r="A18" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="90">
+      <c r="A19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="126">
+      <c r="A20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="162">
+      <c r="A21" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+      <formula1>"Fix, Double check"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented Deeply Nested Activities check.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD446940-8B3A-4025-8F40-ABB2C3CCD1F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3B3793-01C4-4B6C-AAB6-DA5508D4856B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -566,7 +566,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{FACCEB44-97B3-401B-BD48-08626DAD862C}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -847,19 +847,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" style="1"/>
-    <col min="2" max="2" width="15.58203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="28.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.58203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.58203125" style="1"/>
+    <col min="1" max="1" width="8.625" style="1"/>
+    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="28.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>
@@ -906,7 +906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="72">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
@@ -927,7 +927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="90">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
@@ -948,7 +948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="126">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
@@ -969,7 +969,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="144">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="9" t="s">
         <v>62</v>
       </c>
@@ -992,7 +992,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="144">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="9" t="s">
         <v>62</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="144">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="9" t="s">
         <v>62</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="144">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="9" t="s">
         <v>62</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="162">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="9" t="s">
         <v>62</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="180">
+    <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="9" t="s">
         <v>62</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90">
+    <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="9" t="s">
         <v>62</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="54">
+    <row r="13" spans="1:7" ht="56.25">
       <c r="A13" s="9" t="s">
         <v>76</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="54">
+    <row r="14" spans="1:7" ht="75">
       <c r="A14" s="9" t="s">
         <v>67</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="72">
+    <row r="15" spans="1:7" ht="75">
       <c r="A15" s="9" t="s">
         <v>67</v>
       </c>
@@ -1185,9 +1185,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="108">
+    <row r="16" spans="1:7" ht="112.5">
       <c r="A16" s="9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>79</v>
@@ -1208,7 +1208,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="126">
+    <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
         <v>76</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="90">
+    <row r="18" spans="1:7" ht="93.75">
       <c r="A18" s="9" t="s">
         <v>76</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="90">
+    <row r="19" spans="1:7" ht="93.75">
       <c r="A19" s="9" t="s">
         <v>76</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="126">
+    <row r="20" spans="1:7" ht="150">
       <c r="A20" s="9" t="s">
         <v>91</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="162">
+    <row r="21" spans="1:7" ht="168.75">
       <c r="A21" s="9" t="s">
         <v>91</v>
       </c>
@@ -1336,14 +1336,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="49.83203125" customWidth="1"/>
-    <col min="7" max="7" width="40.08203125" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="4" max="5" width="28.375" customWidth="1"/>
+    <col min="6" max="6" width="49.875" customWidth="1"/>
+    <col min="7" max="7" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1369,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Added Japanese localization for more checks.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3B3793-01C4-4B6C-AAB6-DA5508D4856B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43312415-A2DD-4D4E-8916-8BE05FDE4C33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,7 +566,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{FACCEB44-97B3-401B-BD48-08626DAD862C}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -847,19 +847,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="28.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="1"/>
+    <col min="1" max="1" width="8.58203125" style="1"/>
+    <col min="2" max="2" width="15.58203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="28.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.58203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -885,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>
@@ -906,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="72">
       <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
@@ -927,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
@@ -948,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="126">
       <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
@@ -969,7 +967,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A6" s="9" t="s">
         <v>62</v>
       </c>
@@ -992,7 +990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A7" s="9" t="s">
         <v>62</v>
       </c>
@@ -1015,7 +1013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A8" s="9" t="s">
         <v>62</v>
       </c>
@@ -1036,7 +1034,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A9" s="9" t="s">
         <v>62</v>
       </c>
@@ -1057,7 +1055,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="162">
       <c r="A10" s="9" t="s">
         <v>62</v>
       </c>
@@ -1080,7 +1078,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="187.5">
+    <row r="11" spans="1:7" ht="180">
       <c r="A11" s="9" t="s">
         <v>62</v>
       </c>
@@ -1101,7 +1099,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="93.75">
+    <row r="12" spans="1:7" ht="90">
       <c r="A12" s="9" t="s">
         <v>62</v>
       </c>
@@ -1122,7 +1120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="56.25">
+    <row r="13" spans="1:7" ht="54">
       <c r="A13" s="9" t="s">
         <v>76</v>
       </c>
@@ -1143,7 +1141,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75">
+    <row r="14" spans="1:7" ht="54">
       <c r="A14" s="9" t="s">
         <v>67</v>
       </c>
@@ -1164,7 +1162,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="75">
+    <row r="15" spans="1:7" ht="72">
       <c r="A15" s="9" t="s">
         <v>67</v>
       </c>
@@ -1185,7 +1183,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="112.5">
+    <row r="16" spans="1:7" ht="108">
       <c r="A16" s="9" t="s">
         <v>67</v>
       </c>
@@ -1208,7 +1206,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="131.25">
+    <row r="17" spans="1:7" ht="126">
       <c r="A17" s="9" t="s">
         <v>76</v>
       </c>
@@ -1229,7 +1227,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="93.75">
+    <row r="18" spans="1:7" ht="90">
       <c r="A18" s="9" t="s">
         <v>76</v>
       </c>
@@ -1250,7 +1248,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="93.75">
+    <row r="19" spans="1:7" ht="90">
       <c r="A19" s="9" t="s">
         <v>76</v>
       </c>
@@ -1271,7 +1269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="150">
+    <row r="20" spans="1:7" ht="126">
       <c r="A20" s="9" t="s">
         <v>91</v>
       </c>
@@ -1292,7 +1290,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="168.75">
+    <row r="21" spans="1:7" ht="162">
       <c r="A21" s="9" t="s">
         <v>91</v>
       </c>
@@ -1336,14 +1334,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="5" width="28.375" customWidth="1"/>
-    <col min="6" max="6" width="49.875" customWidth="1"/>
-    <col min="7" max="7" width="40.125" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="49.83203125" customWidth="1"/>
+    <col min="7" max="7" width="40.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1369,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Removed duplicated row in config files.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43312415-A2DD-4D4E-8916-8BE05FDE4C33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57179C7E-6C1F-4E39-9B52-C3DFAB56187E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="100">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -845,7 +845,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1248,76 +1248,55 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="90">
+    <row r="19" spans="1:7" ht="126">
       <c r="A19" s="9" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
         <v>77</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="126">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="162">
       <c r="A20" s="9" t="s">
         <v>91</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
         <v>77</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="162">
-      <c r="A21" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="4" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Minor changes to make the WI pass its own checks.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43312415-A2DD-4D4E-8916-8BE05FDE4C33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502205CA-4F89-46CB-B0CE-8278883DD038}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,7 +566,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{FACCEB44-97B3-401B-BD48-08626DAD862C}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -849,15 +849,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" style="1"/>
-    <col min="2" max="2" width="15.58203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="28.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.58203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.58203125" style="1"/>
+    <col min="1" max="1" width="8.625" style="1"/>
+    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="28.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -883,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>
@@ -904,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="72">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
@@ -925,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="90">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="9" t="s">
         <v>62</v>
       </c>
@@ -946,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="126">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="9" t="s">
         <v>62</v>
       </c>
@@ -967,7 +967,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="144">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="9" t="s">
         <v>62</v>
       </c>
@@ -990,7 +990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="144">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="9" t="s">
         <v>62</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="144">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="9" t="s">
         <v>62</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="144">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="9" t="s">
         <v>62</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="162">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="9" t="s">
         <v>62</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="180">
+    <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="9" t="s">
         <v>62</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90">
+    <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="9" t="s">
         <v>62</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="54">
+    <row r="13" spans="1:7" ht="56.25">
       <c r="A13" s="9" t="s">
         <v>76</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="54">
+    <row r="14" spans="1:7" ht="75">
       <c r="A14" s="9" t="s">
         <v>67</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="72">
+    <row r="15" spans="1:7" ht="75">
       <c r="A15" s="9" t="s">
         <v>67</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="108">
+    <row r="16" spans="1:7" ht="112.5">
       <c r="A16" s="9" t="s">
         <v>67</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>80</v>
       </c>
       <c r="D16" s="6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>77</v>
@@ -1206,7 +1206,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="126">
+    <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
         <v>76</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="90">
+    <row r="18" spans="1:7" ht="93.75">
       <c r="A18" s="9" t="s">
         <v>76</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="90">
+    <row r="19" spans="1:7" ht="93.75">
       <c r="A19" s="9" t="s">
         <v>76</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="126">
+    <row r="20" spans="1:7" ht="150">
       <c r="A20" s="9" t="s">
         <v>91</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="162">
+    <row r="21" spans="1:7" ht="168.75">
       <c r="A21" s="9" t="s">
         <v>91</v>
       </c>
@@ -1334,14 +1334,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="49.83203125" customWidth="1"/>
-    <col min="7" max="7" width="40.08203125" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="4" max="5" width="28.375" customWidth="1"/>
+    <col min="6" max="6" width="49.875" customWidth="1"/>
+    <col min="7" max="7" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1367,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Implemented check for repeated activity names.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150CB690-89D3-4E94-9CA8-639032EB19C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF17AE3-D1B2-47C0-9962-B423C998F16A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -278,9 +278,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Variable overrides variable</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -363,10 +360,6 @@
   </si>
   <si>
     <t>Consider the use of Open Browser instead of Open Application or Start Process.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>No</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -847,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
@@ -887,7 +880,7 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
@@ -908,7 +901,7 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
@@ -929,7 +922,7 @@
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>11</v>
@@ -950,7 +943,7 @@
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
@@ -971,7 +964,7 @@
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>16</v>
@@ -994,7 +987,7 @@
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>20</v>
@@ -1017,7 +1010,7 @@
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>43</v>
@@ -1027,7 +1020,7 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>39</v>
@@ -1038,7 +1031,7 @@
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>42</v>
@@ -1048,7 +1041,7 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>40</v>
@@ -1059,7 +1052,7 @@
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>26</v>
@@ -1071,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>24</v>
@@ -1082,7 +1075,7 @@
     </row>
     <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>34</v>
@@ -1092,7 +1085,7 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>33</v>
@@ -1103,7 +1096,7 @@
     </row>
     <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>44</v>
@@ -1113,7 +1106,7 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>36</v>
@@ -1124,7 +1117,7 @@
     </row>
     <row r="13" spans="1:7" ht="56.25">
       <c r="A13" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>63</v>
@@ -1134,7 +1127,7 @@
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>64</v>
@@ -1145,160 +1138,162 @@
     </row>
     <row r="14" spans="1:7" ht="75">
       <c r="A14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75">
       <c r="A15" s="9" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="112.5">
       <c r="A16" s="9" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D16" s="6">
         <v>10</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="93.75">
       <c r="A17" s="9" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="150">
       <c r="A18" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="168.75">
       <c r="A19" s="9" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="131.25">
       <c r="A20" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A16 A17:A20" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16 E17:E20" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Implemented check for repeated workflow name.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF17AE3-D1B2-47C0-9962-B423C998F16A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0518E597-A257-403C-9BA9-080EF68A7D8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -214,188 +214,224 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
+    <t>Check Filename</t>
+  </si>
+  <si>
+    <t>Checks\MissingWorkflowAnnotation.xaml</t>
+  </si>
+  <si>
+    <t>Checks\MissingScreenshot.xaml</t>
+  </si>
+  <si>
+    <t>Checks\UndocumentedDelay.xaml</t>
+  </si>
+  <si>
+    <t>Checks\EmptyCatchBlock.xaml</t>
+  </si>
+  <si>
+    <t>Checks\VariableNamingConvention.xaml</t>
+  </si>
+  <si>
+    <t>Checks\ArgumentNamingConvention.xaml</t>
+  </si>
+  <si>
+    <t>Checks\UndocumentedDefaultClick.xaml</t>
+  </si>
+  <si>
+    <t>Checks\UndocumentedDefaultType.xaml</t>
+  </si>
+  <si>
+    <t>Checks\LargeIdxInSelector.xaml</t>
+  </si>
+  <si>
+    <t>Checks\UnnecessarySequenceOrFlowchart.xaml</t>
+  </si>
+  <si>
+    <t>Checks\UndocumentedUnreachableActivities.xaml</t>
+  </si>
+  <si>
+    <t>Checks\ProjectJsonConfigurationFile.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Variable scope is not the innermost</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Restrict the scope of the variable.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\VariableMinimumScope\VariableMinimumScope.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Variable overrides variable</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\VariableOverridesVariable.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Although it is technically possible for two variables to have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Define unique names for variables, even if they are in different scopes.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Variable overrides argument</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\VariableOverridesArgument.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Although it is technically possible for a variable and an argument have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Define unique names for variables and arguments.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Fix</t>
+  </si>
+  <si>
     <t>Double check</t>
+  </si>
+  <si>
+    <t>Deeply nested activities</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\DeeplyNestedActivities.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>It is usually more difficult to see and understand workflows that have too many deeply nested activities, so it is recommended to avoid deeply nested structures. Instead, it might be better to separate the workflow into smaller ones and use the Invoke Workflow File activity to call them.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Consider dividing the workflow into smaller components to avoid deeply nested structures.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Unused variables</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Workflows should only have variables and arguments that are necessary for its execution. Unused variables and arguments make the project more difficult to understand and should be removed. For removing all unsed variables, use the button "Remove Unused Variables" in UiPath Studio (https://studio.uipath.com/docs/managing-variables#section-removing-variables)</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Remove variables and arguments that are not being used.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Open Browser not being used</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>The Open Browser activity provides a convenient way to open a browser tab or window, and it also serves as a container for activities related to web automation. For this reason, it should be the preferred way to work with browsers, instead of Open Application or Start Process.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Consider the use of Open Browser instead of Open Application or Start Process.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Hotkey without selector</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\HotkeyWithoutSelector.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Send Hotkey activities without selector can be intercepted by any application that comes to the foreground (for example, Windows notifications and antivirus popups), which will prevent the intended execution. For this reason, it is recommended to use selectors or include them in containers that have selectors (for example, Attach Window or Attach Browser).</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Specify a selector when using Send Hotkey activity or include it inside a container.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\RepeatedActivitiyName.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>The names of the activities should give a clear idea of how it is being used. Although the default names usually provide a good description, sometimes they are too generic, so it is recommended to add more information when the context is not clear. This check looks for activities that have the same name, which might indicate that the same generic name is used multiple times. The check accepts an argument which is the threshold of how many activities can have the same name.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Check if it could be easier to understand what the activity does by adding a more descriptive title.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\OpenBrowserNotUsed.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Workflows in a project should have unique names (even if they are in different folders) to facilitate project organization and debugging.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Make the name of the workflow unique within a project.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Empty Then block</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\EmptyThenBlock.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Redefine the condition so that actions are taken in the Then block.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>In an If activity, it is recommended to define the condition so that the Then block is always used. Having an empty Then block (and actions performed in the Else block) makes the workflow harder to understand.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\RepeatedWorkflowName.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Repeated workflow name</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Check Filename</t>
-  </si>
-  <si>
-    <t>Checks\MissingWorkflowAnnotation.xaml</t>
-  </si>
-  <si>
-    <t>Checks\MissingScreenshot.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDelay.xaml</t>
-  </si>
-  <si>
-    <t>Checks\EmptyCatchBlock.xaml</t>
-  </si>
-  <si>
-    <t>Checks\VariableNamingConvention.xaml</t>
-  </si>
-  <si>
-    <t>Checks\ArgumentNamingConvention.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDefaultClick.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDefaultType.xaml</t>
-  </si>
-  <si>
-    <t>Checks\LargeIdxInSelector.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UnnecessarySequenceOrFlowchart.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UndocumentedUnreachableActivities.xaml</t>
-  </si>
-  <si>
-    <t>Checks\ProjectJsonConfigurationFile.xaml</t>
+    <t>Repeated activity display name</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\RepeatedActivityName.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Yes</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variable scope is not the innermost</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Restrict the scope of the variable.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\VariableMinimumScope\VariableMinimumScope.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variable overrides variable</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\VariableOverridesVariable.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Although it is technically possible for two variables to have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Define unique names for variables, even if they are in different scopes.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variable overrides argument</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\VariableOverridesArgument.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Although it is technically possible for a variable and an argument have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Define unique names for variables and arguments.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Fix</t>
-  </si>
-  <si>
-    <t>Double check</t>
-  </si>
-  <si>
-    <t>Deeply nested activities</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\DeeplyNestedActivities.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>It is usually more difficult to see and understand workflows that have too many deeply nested activities, so it is recommended to avoid deeply nested structures. Instead, it might be better to separate the workflow into smaller ones and use the Invoke Workflow File activity to call them.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Consider dividing the workflow into smaller components to avoid deeply nested structures.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Unused variables</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\UnusedVariables.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Workflows should only have variables and arguments that are necessary for its execution. Unused variables and arguments make the project more difficult to understand and should be removed. For removing all unsed variables, use the button "Remove Unused Variables" in UiPath Studio (https://studio.uipath.com/docs/managing-variables#section-removing-variables)</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Remove variables and arguments that are not being used.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Open Browser not being used</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>The Open Browser activity provides a convenient way to open a browser tab or window, and it also serves as a container for activities related to web automation. For this reason, it should be the preferred way to work with browsers, instead of Open Application or Start Process.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Consider the use of Open Browser instead of Open Application or Start Process.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Hotkey without selector</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\HotkeyWithoutSelector.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Send Hotkey activities without selector can be intercepted by any application that comes to the foreground (for example, Windows notifications and antivirus popups), which will prevent the intended execution. For this reason, it is recommended to use selectors or include them in containers that have selectors (for example, Attach Window or Attach Browser).</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Specify a selector when using Send Hotkey activity or include it inside a container.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Repeated display names for activities</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\RepeatedActivitiyName.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>The names of the activities should give a clear idea of how it is being used. Although the default names usually provide a good description, sometimes they are too generic, so it is recommended to add more information when the context is not clear. This check looks for activities that have the same name, which might indicate that the same generic name is used multiple times. The check accepts an argument which is the threshold of how many activities can have the same name.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Check if it could be easier to understand what the activity does by adding a more descriptive title.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\OpenBrowserNotUsed.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -838,11 +874,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -863,7 +897,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -880,13 +914,13 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -901,13 +935,13 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -922,13 +956,13 @@
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
@@ -943,13 +977,13 @@
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
@@ -964,13 +998,13 @@
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>19</v>
@@ -987,13 +1021,13 @@
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>23</v>
@@ -1010,17 +1044,17 @@
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>39</v>
@@ -1031,17 +1065,17 @@
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>40</v>
@@ -1052,19 +1086,19 @@
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>24</v>
@@ -1075,17 +1109,17 @@
     </row>
     <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>33</v>
@@ -1096,17 +1130,17 @@
     </row>
     <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>36</v>
@@ -1117,183 +1151,204 @@
     </row>
     <row r="13" spans="1:7" ht="56.25">
       <c r="A13" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75">
       <c r="A14" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75">
       <c r="A15" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="112.5">
       <c r="A16" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D16" s="6">
         <v>10</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="93.75">
       <c r="A17" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="150">
       <c r="A18" s="9" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="168.75">
       <c r="A19" s="9" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="131.25">
       <c r="A20" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75">
+      <c r="A21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1304,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1345,17 +1400,17 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>27</v>
@@ -1364,11 +1419,35 @@
         <v>28</v>
       </c>
     </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="56.25">
+      <c r="A3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{FB738567-74EA-496C-A485-98E380BDFD1E}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3" xr:uid="{FB738567-74EA-496C-A485-98E380BDFD1E}">
       <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{4684231F-5ABA-493C-8654-B20DAC346DD1}">
+      <formula1>"Fix, Double check"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added check for empty Then blocks.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0518E597-A257-403C-9BA9-080EF68A7D8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A47F743-F3DD-41AC-A8EA-207A1BE02085}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,23 +395,11 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>No</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Empty Then block</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Checks\EmptyThenBlock.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Redefine the condition so that actions are taken in the Then block.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>In an If activity, it is recommended to define the condition so that the Then block is always used. Having an empty Then block (and actions performed in the Else block) makes the workflow harder to understand.</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -433,6 +421,17 @@
   <si>
     <t>Yes</t>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>In an If activity (or FlowDecision activity), it is recommended to define the condition so that the Then block (True branch) is always used. Having an empty Then block (True branch) makes the workflow harder to understand.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Redefine the condition so that actions are taken in the Then block (True branch, in case of FlowDecision).</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -876,7 +875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -914,7 +915,7 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
@@ -935,7 +936,7 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
@@ -956,7 +957,7 @@
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>11</v>
@@ -977,7 +978,7 @@
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
@@ -998,7 +999,7 @@
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>16</v>
@@ -1021,7 +1022,7 @@
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>20</v>
@@ -1044,7 +1045,7 @@
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>43</v>
@@ -1065,7 +1066,7 @@
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>42</v>
@@ -1086,7 +1087,7 @@
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>26</v>
@@ -1109,7 +1110,7 @@
     </row>
     <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>34</v>
@@ -1130,7 +1131,7 @@
     </row>
     <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>44</v>
@@ -1172,7 +1173,7 @@
     </row>
     <row r="14" spans="1:7" ht="75">
       <c r="A14" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>66</v>
@@ -1193,7 +1194,7 @@
     </row>
     <row r="15" spans="1:7" ht="75">
       <c r="A15" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>70</v>
@@ -1214,7 +1215,7 @@
     </row>
     <row r="16" spans="1:7" ht="112.5">
       <c r="A16" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>77</v>
@@ -1237,7 +1238,7 @@
     </row>
     <row r="17" spans="1:7" ht="93.75">
       <c r="A17" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>84</v>
@@ -1258,7 +1259,7 @@
     </row>
     <row r="18" spans="1:7" ht="150">
       <c r="A18" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>87</v>
@@ -1279,10 +1280,10 @@
     </row>
     <row r="19" spans="1:7" ht="168.75">
       <c r="A19" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>91</v>
@@ -1308,7 +1309,7 @@
         <v>81</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
@@ -1321,25 +1322,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75">
+    <row r="21" spans="1:7" ht="93.75">
       <c r="A21" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
         <v>75</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1424,10 +1425,10 @@
         <v>61</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">

</xml_diff>

<commit_message>
Divide checks in folders (standard and custom).
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A47F743-F3DD-41AC-A8EA-207A1BE02085}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B900E0-D493-474B-AF9D-38121E722F6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19410" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -217,43 +217,6 @@
     <t>Check Filename</t>
   </si>
   <si>
-    <t>Checks\MissingWorkflowAnnotation.xaml</t>
-  </si>
-  <si>
-    <t>Checks\MissingScreenshot.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDelay.xaml</t>
-  </si>
-  <si>
-    <t>Checks\EmptyCatchBlock.xaml</t>
-  </si>
-  <si>
-    <t>Checks\VariableNamingConvention.xaml</t>
-  </si>
-  <si>
-    <t>Checks\ArgumentNamingConvention.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDefaultClick.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UndocumentedDefaultType.xaml</t>
-  </si>
-  <si>
-    <t>Checks\LargeIdxInSelector.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UnnecessarySequenceOrFlowchart.xaml</t>
-  </si>
-  <si>
-    <t>Checks\UndocumentedUnreachableActivities.xaml</t>
-  </si>
-  <si>
-    <t>Checks\ProjectJsonConfigurationFile.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Yes</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -270,18 +233,10 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\VariableMinimumScope\VariableMinimumScope.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Variable overrides variable</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\VariableOverridesVariable.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Although it is technically possible for two variables to have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -294,10 +249,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\VariableOverridesArgument.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Although it is technically possible for a variable and an argument have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -319,10 +270,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\DeeplyNestedActivities.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>It is usually more difficult to see and understand workflows that have too many deeply nested activities, so it is recommended to avoid deeply nested structures. Instead, it might be better to separate the workflow into smaller ones and use the Invoke Workflow File activity to call them.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -359,10 +306,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\HotkeyWithoutSelector.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Send Hotkey activities without selector can be intercepted by any application that comes to the foreground (for example, Windows notifications and antivirus popups), which will prevent the intended execution. For this reason, it is recommended to use selectors or include them in containers that have selectors (for example, Attach Window or Attach Browser).</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -371,10 +314,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\RepeatedActivitiyName.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>The names of the activities should give a clear idea of how it is being used. Although the default names usually provide a good description, sometimes they are too generic, so it is recommended to add more information when the context is not clear. This check looks for activities that have the same name, which might indicate that the same generic name is used multiple times. The check accepts an argument which is the threshold of how many activities can have the same name.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -383,10 +322,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\OpenBrowserNotUsed.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Workflows in a project should have unique names (even if they are in different folders) to facilitate project organization and debugging.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -396,14 +331,6 @@
   </si>
   <si>
     <t>Empty Then block</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\EmptyThenBlock.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\RepeatedWorkflowName.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -415,10 +342,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\RepeatedActivityName.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Yes</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -432,6 +355,94 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Checks\Standard\MissingWorkflowAnnotation.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\MissingScreenshot.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\UndocumentedDelay.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\EmptyCatchBlock.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\VariableNamingConvention.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\ArgumentNamingConvention.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\UndocumentedDefaultClick.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\UndocumentedDefaultType.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\LargeIdxInSelector.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\UnnecessarySequenceOrFlowchart.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\UndocumentedUnreachableActivities.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\DeeplyNestedActivities.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\OpenBrowserNotUsed.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\HotkeyWithoutSelector.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\RepeatedActivitiyName.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\UnusedVariables.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\EmptyThenBlock.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\ProjectJsonConfigurationFile.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\RepeatedWorkflowName.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Custom\VariableOverridesArgument.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Custom\VariableOverridesVariable.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Custom\VariableMinimumScope\VariableMinimumScope.xaml</t>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -875,9 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -915,13 +924,13 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -936,13 +945,13 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -957,13 +966,13 @@
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
@@ -978,13 +987,13 @@
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
@@ -999,13 +1008,13 @@
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>19</v>
@@ -1022,13 +1031,13 @@
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>23</v>
@@ -1045,17 +1054,17 @@
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>39</v>
@@ -1066,17 +1075,17 @@
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>40</v>
@@ -1087,19 +1096,19 @@
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>24</v>
@@ -1110,17 +1119,17 @@
     </row>
     <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>33</v>
@@ -1131,17 +1140,17 @@
     </row>
     <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>36</v>
@@ -1150,61 +1159,63 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="56.25">
+    <row r="13" spans="1:7" ht="112.5">
       <c r="A13" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="9"/>
+      <c r="C13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="6">
+        <v>10</v>
+      </c>
       <c r="E13" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75">
+    <row r="14" spans="1:7" ht="93.75">
       <c r="A14" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="75">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="150">
       <c r="A15" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>72</v>
@@ -1213,143 +1224,141 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="112.5">
+    <row r="16" spans="1:7" ht="168.75">
       <c r="A16" s="9" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="D16" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="93.75">
+    </row>
+    <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="150">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="93.75">
       <c r="A18" s="9" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="168.75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="75">
       <c r="A19" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="9"/>
       <c r="E19" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="131.25">
+        <v>60</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="75">
       <c r="A20" s="9" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="93.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75">
       <c r="A21" s="9" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A12 A13:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E12 E13:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1362,9 +1371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1401,17 +1408,17 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>27</v>
@@ -1422,23 +1429,23 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="56.25">
       <c r="A3" s="9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed argument parsing mechanism to accept JSON strings in the configuration file.
The JSON file is converted to a dictionary for easier manipulation within a check. This required a change in the in_CheckArgument argument's type (from String to Dictionary(Of String, String)). Also, the in_CheckArgument argument was renamed to in_CheckArguments.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B900E0-D493-474B-AF9D-38121E722F6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD359BA0-2135-4121-BA5C-001D7565AEA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19410" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="111">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -99,10 +99,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>(^(dt_)*([A-Z][a-z0-9]*)+$)</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>Arguments not following naming convention</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -113,10 +109,6 @@
   <si>
     <t>Arguments in a project should follow a specified naming convention, since it makes it easier to understand the project and maintain it. This check receives a regular expression that dictates the naming convention for arguments. For more information about naming conventions, refer to https://studio.uipath.com/docs/workflow-design#section-naming-conventions</t>
     <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>(^(in_|out_|io_)(dt_)*([A-Z][a-z0-9]*)+)</t>
-    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>The idx attribute is used to distinguish elements with the same selector based on their order in the interface hierarchy. This order can change if the elements on the screen change, so the value for the idx attribute should be kept to a low value to avoid the selection of wrong elements. This checks receives a threshold for the value of the idx attribute. For more about selectors, refer to https://studio.uipath.com/docs/ui-automation#section-selectors</t>
@@ -443,6 +435,40 @@
   <si>
     <t>Checks\Custom\VariableMinimumScope\VariableMinimumScope.xaml</t>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>{
+"Threshold" : "1"
+}</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>{
+"Threshold" : "10"
+}</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>{
+"Threshold" : "2"
+}</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>{ 
+"NamingPattern" : "(^(dt_)*([A-Z][a-z0-9]*)+$)"
+}</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>{ 
+"NamingPattern" : "(^(in_|out_|io_)(dt_)*([A-Z][a-z0-9]*)+)"
+}</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Arguments</t>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
@@ -901,19 +927,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -924,17 +950,17 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
@@ -945,17 +971,17 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
@@ -966,17 +992,17 @@
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>13</v>
@@ -987,40 +1013,40 @@
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>19</v>
+        <v>87</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>18</v>
@@ -1031,325 +1057,325 @@
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
+        <v>91</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="112.5">
       <c r="A13" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="6">
-        <v>10</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="93.75">
       <c r="A14" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="150">
       <c r="A15" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="168.75">
       <c r="A16" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="93.75">
       <c r="A18" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="75">
       <c r="A19" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="75">
       <c r="A20" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="75">
       <c r="A21" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1385,10 +1411,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>
@@ -1397,7 +1423,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1408,44 +1434,44 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="56.25">
       <c r="A3" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typos in checklists.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD359BA0-2135-4121-BA5C-001D7565AEA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAFDDCE-0049-4867-B8AD-C0DE17548084}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19410" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -405,10 +405,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Checks\Standard\RepeatedActivitiyName.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\Standard\UnusedVariables.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -469,6 +465,10 @@
   <si>
     <t>Arguments</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Checks\Standard\RepeatedActivityName.xaml</t>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -936,7 +936,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -1043,7 +1043,7 @@
         <v>87</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>45</v>
@@ -1066,7 +1066,7 @@
         <v>88</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>45</v>
@@ -1131,7 +1131,7 @@
         <v>91</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>59</v>
@@ -1196,7 +1196,7 @@
         <v>94</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>58</v>
@@ -1258,10 +1258,10 @@
         <v>78</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>58</v>
@@ -1275,13 +1275,13 @@
     </row>
     <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
@@ -1302,7 +1302,7 @@
         <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
@@ -1317,13 +1317,13 @@
     </row>
     <row r="19" spans="1:7" ht="75">
       <c r="A19" s="9" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="6" t="s">
@@ -1344,7 +1344,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
@@ -1365,7 +1365,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
@@ -1440,7 +1440,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -1461,7 +1461,7 @@
         <v>77</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">

</xml_diff>

<commit_message>
Turned on all checks.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAFDDCE-0049-4867-B8AD-C0DE17548084}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F014A8FD-A822-43C2-8005-B0B2C1E5DB9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="109">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -249,9 +249,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Fix</t>
   </si>
   <si>
@@ -334,10 +331,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Yes</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>In an If activity (or FlowDecision activity), it is recommended to define the condition so that the Then block (True branch) is always used. Having an empty Then block (True branch) makes the workflow harder to understand.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -346,9 +339,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Checks\Standard\MissingWorkflowAnnotation.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -402,10 +392,6 @@
   </si>
   <si>
     <t>Checks\Standard\HotkeyWithoutSelector.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\Standard\UnusedVariables.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -468,6 +454,14 @@
   </si>
   <si>
     <t>Checks\Standard\RepeatedActivityName.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\UnusedVariables\UnusedVariables.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -936,7 +930,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -950,13 +944,13 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A2" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -971,13 +965,13 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
       <c r="A3" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -992,13 +986,13 @@
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A4" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
@@ -1013,13 +1007,13 @@
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A5" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
@@ -1034,16 +1028,16 @@
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A6" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>45</v>
@@ -1057,16 +1051,16 @@
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A7" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>45</v>
@@ -1080,17 +1074,17 @@
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A8" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>37</v>
@@ -1101,17 +1095,17 @@
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A9" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>38</v>
@@ -1122,19 +1116,19 @@
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A10" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>22</v>
@@ -1145,17 +1139,17 @@
     </row>
     <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>31</v>
@@ -1166,17 +1160,17 @@
     </row>
     <row r="12" spans="1:7" ht="93.75">
       <c r="A12" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>34</v>
@@ -1187,147 +1181,147 @@
     </row>
     <row r="13" spans="1:7" ht="112.5">
       <c r="A13" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="93.75">
       <c r="A14" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="150">
       <c r="A15" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="168.75">
       <c r="A16" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="93.75">
       <c r="A18" s="9" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="75">
       <c r="A19" s="9" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>49</v>
@@ -1338,17 +1332,17 @@
     </row>
     <row r="20" spans="1:7" ht="75">
       <c r="A20" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>52</v>
@@ -1359,17 +1353,17 @@
     </row>
     <row r="21" spans="1:7" ht="75">
       <c r="A21" s="9" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>55</v>
@@ -1381,10 +1375,10 @@
   </sheetData>
   <phoneticPr fontId="6"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A12 A13:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E12 E13:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1440,11 +1434,11 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>25</v>
@@ -1458,20 +1452,20 @@
         <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented the possibility for the check for hotkeys without selectos to accept UIElements.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F014A8FD-A822-43C2-8005-B0B2C1E5DB9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2885F6-9D4F-4185-90F2-7A3A869B469F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -295,10 +295,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Send Hotkey activities without selector can be intercepted by any application that comes to the foreground (for example, Windows notifications and antivirus popups), which will prevent the intended execution. For this reason, it is recommended to use selectors or include them in containers that have selectors (for example, Attach Window or Attach Browser).</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Specify a selector when using Send Hotkey activity or include it inside a container.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -462,6 +458,10 @@
   </si>
   <si>
     <t>Checks\Standard\UnusedVariables\UnusedVariables.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Send Hotkey activities without selectors or specified UI elements can be intercepted by any application that comes to the foreground (for example, Windows notifications and antivirus popups), which will prevent the intended execution. For this reason, it is recommended to use selectors or include them in containers that have selectors (for example, Attach Window or Attach Browser).</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -906,7 +906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -930,7 +932,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -950,7 +952,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -971,7 +973,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -992,7 +994,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
@@ -1013,7 +1015,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
@@ -1034,10 +1036,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>45</v>
@@ -1057,10 +1059,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>45</v>
@@ -1080,7 +1082,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
@@ -1101,7 +1103,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
@@ -1122,10 +1124,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>58</v>
@@ -1145,7 +1147,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
@@ -1166,7 +1168,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
@@ -1187,10 +1189,10 @@
         <v>59</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>57</v>
@@ -1210,7 +1212,7 @@
         <v>65</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
@@ -1231,17 +1233,17 @@
         <v>68</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="168.75">
@@ -1249,33 +1251,33 @@
         <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
@@ -1290,23 +1292,23 @@
     </row>
     <row r="18" spans="1:7" ht="93.75">
       <c r="A18" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="75">
@@ -1317,7 +1319,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="6" t="s">
@@ -1338,7 +1340,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
@@ -1359,7 +1361,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
@@ -1434,7 +1436,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -1452,20 +1454,20 @@
         <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standardized annotations and naming of variables, arguments adn activities.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2885F6-9D4F-4185-90F2-7A3A869B469F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80611D1-725C-405E-B2B7-BD0E15147D0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,10 +283,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>The Open Browser activity provides a convenient way to open a browser tab or window, and it also serves as a container for activities related to web automation. For this reason, it should be the preferred way to work with browsers, instead of Open Application or Start Process.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Consider the use of Open Browser instead of Open Application or Start Process.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -462,6 +458,10 @@
   </si>
   <si>
     <t>Send Hotkey activities without selectors or specified UI elements can be intercepted by any application that comes to the foreground (for example, Windows notifications and antivirus popups), which will prevent the intended execution. For this reason, it is recommended to use selectors or include them in containers that have selectors (for example, Attach Window or Attach Browser).</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>The Open Browser activity provides a convenient way to open a browser tab or window, and it also serves as a container for activities related to web automation. For this reason, it is the preferred way to work with browsers, instead of Open Application or Start Process.</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
@@ -932,7 +932,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -952,7 +952,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -973,7 +973,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -994,7 +994,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
@@ -1015,7 +1015,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
@@ -1036,10 +1036,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>45</v>
@@ -1059,10 +1059,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>45</v>
@@ -1082,7 +1082,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
@@ -1103,7 +1103,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
@@ -1124,10 +1124,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>58</v>
@@ -1147,7 +1147,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
@@ -1168,7 +1168,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
@@ -1189,10 +1189,10 @@
         <v>59</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>57</v>
@@ -1212,17 +1212,17 @@
         <v>65</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="150">
@@ -1230,20 +1230,20 @@
         <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="168.75">
@@ -1251,33 +1251,33 @@
         <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
@@ -1292,23 +1292,23 @@
     </row>
     <row r="18" spans="1:7" ht="93.75">
       <c r="A18" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="75">
@@ -1319,7 +1319,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="6" t="s">
@@ -1340,7 +1340,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
@@ -1361,7 +1361,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
@@ -1436,7 +1436,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -1454,20 +1454,20 @@
         <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed "Double check" to "Double-check".
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80611D1-725C-405E-B2B7-BD0E15147D0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26047781-3DB8-4616-BD46-60BF3403FFE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -252,9 +252,6 @@
     <t>Fix</t>
   </si>
   <si>
-    <t>Double check</t>
-  </si>
-  <si>
     <t>Deeply nested activities</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -463,6 +460,9 @@
   <si>
     <t>The Open Browser activity provides a convenient way to open a browser tab or window, and it also serves as a container for activities related to web automation. For this reason, it is the preferred way to work with browsers, instead of Open Application or Start Process.</t>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Double-check</t>
   </si>
 </sst>
 </file>
@@ -906,9 +906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -932,7 +930,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -952,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -973,7 +971,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -994,7 +992,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
@@ -1015,7 +1013,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
@@ -1036,10 +1034,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>45</v>
@@ -1059,10 +1057,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>45</v>
@@ -1082,11 +1080,11 @@
         <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>37</v>
@@ -1103,11 +1101,11 @@
         <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>38</v>
@@ -1124,13 +1122,13 @@
         <v>24</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>22</v>
@@ -1147,11 +1145,11 @@
         <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>31</v>
@@ -1168,7 +1166,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
@@ -1186,22 +1184,22 @@
         <v>47</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="93.75">
@@ -1209,20 +1207,20 @@
         <v>47</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="150">
@@ -1230,20 +1228,20 @@
         <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="168.75">
@@ -1251,64 +1249,64 @@
         <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="131.25">
       <c r="A17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="93.75">
       <c r="A18" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="75">
@@ -1319,7 +1317,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="6" t="s">
@@ -1340,7 +1338,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
@@ -1361,7 +1359,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
@@ -1376,12 +1374,15 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 E12:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E11" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
+      <formula1>"Fix, Double-check"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1436,7 +1437,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
@@ -1454,20 +1455,20 @@
         <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included new checks in checklists.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26047781-3DB8-4616-BD46-60BF3403FFE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64E667B-7166-449D-B606-FF459C335858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,9 @@
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
     <sheet name="Project" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Workflow!$A$1:$G$25</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -463,6 +466,86 @@
   </si>
   <si>
     <t>Double-check</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Hardcoded password</t>
+  </si>
+  <si>
+    <t>Checks\Standard\HardcodedPassword.xaml</t>
+  </si>
+  <si>
+    <t>Passwords that are hardcoded into workflows can be a serious security threat since they can be easily recovered by unauthorized parties. For more about protecting sensitive data, please refer to https://docs.uipath.com/studio/docs/protecting-sensitive-information</t>
+  </si>
+  <si>
+    <t>Passwords should be stored in secure locations, like Orchestrator or Windows Credential Manager.</t>
+  </si>
+  <si>
+    <t>Mandatory files in project</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Custom\MandatoryFilesInProject.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>{
+  "MandatoryFiles": "Data\\Config.xlsx,Framework\\CloseAllApplications.xaml,Framework\\GetAppCredentials.xaml,Framework\\GetTransactionData.xaml,Framework\\InitAllApplications.xaml,Framework\\InitAllSettings.xaml,Framework\\KillAllProcesses.xaml,Framework\\SetTransactionStatus.xaml,Framework\\TakeScreenshot.xaml,Main.xaml,Process.xaml"
+}</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>The project should contain mandatory files specified by the COE or project leader. This check receives a list of files that should be in the project folder.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Include mandatory files in the project folder.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Undocumented Parallel activity</t>
+  </si>
+  <si>
+    <t>Checks\Standard\UndocumentedParallelActivity.xaml</t>
+  </si>
+  <si>
+    <t>Using the Parallel activity can make the workflow harder to understand and might lead to unexpected results when combined with UI interactions. If it is necessary to use the Parallel activity, include an annotation to explain the situation.
+For more about the Parallel activity, please refer to https://docs.microsoft.com/en-us/dotnet/api/system.activities.statements.parallel?view=netframework-4.8</t>
+  </si>
+  <si>
+    <t>Verify whether the Parallel activity is really necessary and, if it is, include an annotation explaning why it is being used.</t>
+  </si>
+  <si>
+    <t>Undocumented Image-based activities</t>
+  </si>
+  <si>
+    <t>Checks\Standard\UndocumentedImageBasedActivities.xaml</t>
+  </si>
+  <si>
+    <t>The use of image-based activities (e.g., Click Image and Wait Image Vanish) is not usually recommended, because they are sensitive to screen resolutions and image quality.
+In cases they must be used, it is a good practice to include an annotation to the activity to explain the situation.</t>
+  </si>
+  <si>
+    <t>Confirm whether image-based activities are really necessary and, if they are, add an annotation to explain the situation.</t>
+  </si>
+  <si>
+    <t>Workflow naming convention</t>
+  </si>
+  <si>
+    <t>Checks\Custom\WorkflowFileNamingConvention.xaml</t>
+  </si>
+  <si>
+    <t>{ 
+"NamingPattern" : "^[A-Z0-9]{7}_[0-9]{3}_.*$"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workflows in a project should be named according to the project's naming conventions.  This check receives a regular expression that dictates the naming convention for workflow files. </t>
+  </si>
+  <si>
+    <t>Change the name of the file to match the project's naming conventions.</t>
   </si>
 </sst>
 </file>
@@ -588,7 +671,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -622,6 +705,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -904,7 +993,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -942,155 +1031,153 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="150">
       <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="E2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A3" s="9" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="93.75">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="187.5">
       <c r="A4" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="131.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A5" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="150">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A6" s="9" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>45</v>
+        <v>120</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="150">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A7" s="9" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>45</v>
+        <v>124</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="150">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="93.75">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
@@ -1114,48 +1201,48 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="168.75">
+    <row r="10" spans="1:7" ht="150">
       <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>24</v>
+      <c r="B10" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
         <v>108</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="187.5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="168.75">
       <c r="A11" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="6"/>
+        <v>103</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="E11" s="6" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="93.75">
@@ -1163,226 +1250,317 @@
         <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="112.5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="93.75">
       <c r="A13" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>98</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="93.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75">
       <c r="A14" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="150">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="168.75">
       <c r="A15" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="150">
+      <c r="A16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="168.75">
-      <c r="A16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="131.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="112.5">
       <c r="A17" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="93.75">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.75">
       <c r="A18" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="75">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="131.25">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="D19" s="13"/>
       <c r="E19" s="6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="75">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="112.5">
       <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="6"/>
+      <c r="B20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="150">
+      <c r="A21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="75">
+      <c r="A22" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="75">
+      <c r="A23" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G23" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75">
-      <c r="A21" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="24" spans="1:7" ht="75">
+      <c r="A24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
+      <c r="D24" s="6"/>
+      <c r="E24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="25" spans="1:7" ht="75">
+      <c r="A25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
+    <sortCondition descending="1" ref="C2:C25"/>
+  </sortState>
   <phoneticPr fontId="6"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 E12:E21" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E25 E2:E6" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E11" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E10" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
       <formula1>"Fix, Double-check"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A25" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+      <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1392,9 +1570,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1471,13 +1651,36 @@
         <v>71</v>
       </c>
     </row>
+    <row r="4" spans="1:7" ht="262.5">
+      <c r="A4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3" xr:uid="{FB738567-74EA-496C-A485-98E380BDFD1E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4" xr:uid="{FB738567-74EA-496C-A485-98E380BDFD1E}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{4684231F-5ABA-493C-8654-B20DAC346DD1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{4684231F-5ABA-493C-8654-B20DAC346DD1}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Made some checks into standard checks instead of custom.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64E667B-7166-449D-B606-FF459C335858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B261071-51D7-4367-9E57-6D322969E8AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
     <sheet name="Project" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Workflow!$A$1:$G$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Workflow!$A$1:$G$24</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="133">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -396,18 +396,6 @@
   </si>
   <si>
     <t>Checks\Standard\RepeatedWorkflowName.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\Custom\VariableOverridesArgument.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\Custom\VariableOverridesVariable.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Checks\Custom\VariableMinimumScope\VariableMinimumScope.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -546,6 +534,21 @@
   </si>
   <si>
     <t>Change the name of the file to match the project's naming conventions.</t>
+  </si>
+  <si>
+    <t>Checks\Standard\VariableOverridesVariable.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\VariableOverridesArgument.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Checks\Standard\VariableMinimumScope\VariableMinimumScope.xaml</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -995,7 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -1019,7 +1022,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -1042,7 +1045,7 @@
         <v>81</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>45</v>
@@ -1056,13 +1059,13 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A3" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -1087,7 +1090,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>31</v>
@@ -1119,44 +1122,44 @@
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A6" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A7" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="93.75">
@@ -1192,7 +1195,7 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>38</v>
@@ -1213,7 +1216,7 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>37</v>
@@ -1230,10 +1233,10 @@
         <v>74</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>57</v>
@@ -1260,7 +1263,7 @@
         <v>57</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>65</v>
@@ -1319,10 +1322,10 @@
         <v>85</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>22</v>
@@ -1346,7 +1349,7 @@
         <v>57</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>67</v>
@@ -1354,28 +1357,28 @@
     </row>
     <row r="17" spans="1:7" ht="112.5">
       <c r="A17" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="12" customFormat="1" ht="93.75">
       <c r="A18" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>72</v>
@@ -1426,7 +1429,7 @@
         <v>88</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>57</v>
@@ -1449,7 +1452,7 @@
         <v>82</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>45</v>
@@ -1461,48 +1464,46 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="75">
+    <row r="22" spans="1:7" ht="75">
       <c r="A22" s="9" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="13"/>
+      <c r="E22" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="75">
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="13"/>
+      <c r="B23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>53</v>
+      <c r="F23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="75">
@@ -1510,56 +1511,58 @@
         <v>47</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="6"/>
+        <v>131</v>
+      </c>
+      <c r="D24" s="4"/>
       <c r="E24" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="75">
       <c r="A25" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>50</v>
+      <c r="F25" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
-    <sortCondition descending="1" ref="C2:C25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G24">
+    <sortCondition descending="1" ref="C2:C24"/>
   </sortState>
   <phoneticPr fontId="6"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E25 E2:E6" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E21 E22:E25" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E10" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
       <formula1>"Fix, Double-check"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A25" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A21 A22:A25" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1572,9 +1575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1653,25 +1654,25 @@
     </row>
     <row r="4" spans="1:7" ht="262.5">
       <c r="A4" s="9" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added note about limitation of Variable Minimum Scope check.
Limitation: It can give false alerts for variables binded to InOut argumets inside repetitive structures.
Co-Authored-By: Silviu Predan <silviuui@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B261071-51D7-4367-9E57-6D322969E8AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5423F2D1-8B6C-492E-A42B-3EA2CD9A37EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -220,10 +220,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Restrict the scope of the variable.</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -549,6 +545,11 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.
+Limitation: It can give false alerts for variables binded to InOut argumets inside repetitive structures.</t>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -998,7 +999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -1022,7 +1023,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -1042,10 +1043,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>45</v>
@@ -1059,23 +1060,23 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A3" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="187.5">
@@ -1086,11 +1087,11 @@
         <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>31</v>
@@ -1107,11 +1108,11 @@
         <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>34</v>
@@ -1122,44 +1123,44 @@
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="168.75">
       <c r="A6" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="131.25">
       <c r="A7" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="93.75">
@@ -1170,7 +1171,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
@@ -1191,11 +1192,11 @@
         <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>38</v>
@@ -1212,11 +1213,11 @@
         <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>37</v>
@@ -1230,22 +1231,22 @@
         <v>47</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="93.75">
@@ -1253,20 +1254,20 @@
         <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="93.75">
@@ -1277,7 +1278,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
@@ -1298,7 +1299,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
@@ -1319,13 +1320,13 @@
         <v>24</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>22</v>
@@ -1339,62 +1340,62 @@
         <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="112.5">
       <c r="A17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="12" customFormat="1" ht="93.75">
       <c r="A18" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="12" customFormat="1" ht="131.25">
@@ -1405,7 +1406,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="6" t="s">
@@ -1423,22 +1424,22 @@
         <v>47</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="12" customFormat="1" ht="150">
@@ -1449,10 +1450,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>45</v>
@@ -1469,20 +1470,20 @@
         <v>47</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="75">
@@ -1490,23 +1491,23 @@
         <v>47</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="75">
+    </row>
+    <row r="24" spans="1:7" ht="93.75">
       <c r="A24" s="9" t="s">
         <v>47</v>
       </c>
@@ -1514,40 +1515,40 @@
         <v>48</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="12" customFormat="1" ht="75">
       <c r="A25" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1618,11 +1619,11 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>25</v>
@@ -1636,43 +1637,43 @@
         <v>47</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="262.5">
       <c r="A4" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified to existing check to support "UiPath Coding Standards and Workflow Quality Evaluation Kit"
1.HardcodedPassword.xaml
Changed to retrieve attribute list to check from argument so that attributes other than "Password" can be checked.

2.ProjectJsonConfigurationFile.xaml
Added the check that the workflow file of "main" parameter of project.json exists.
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5423F2D1-8B6C-492E-A42B-3EA2CD9A37EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{5423F2D1-8B6C-492E-A42B-3EA2CD9A37EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C6314EC5-7066-44DE-82EE-DF71412FA216}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="640" windowWidth="14540" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="134">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -461,9 +461,6 @@
     <t>Checks\Standard\HardcodedPassword.xaml</t>
   </si>
   <si>
-    <t>Passwords that are hardcoded into workflows can be a serious security threat since they can be easily recovered by unauthorized parties. For more about protecting sensitive data, please refer to https://docs.uipath.com/studio/docs/protecting-sensitive-information</t>
-  </si>
-  <si>
     <t>Passwords should be stored in secure locations, like Orchestrator or Windows Credential Manager.</t>
   </si>
   <si>
@@ -549,6 +546,16 @@
   <si>
     <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.
 Limitation: It can give false alerts for variables binded to InOut argumets inside repetitive structures.</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Passwords that are hardcoded into workflows can be a serious security threat since they can be easily recovered by unauthorized parties. This check receives a list of attributes to check for hardcoded. For more about protecting sensitive data, please refer to https://docs.uipath.com/studio/docs/protecting-sensitive-information</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>{
+"Attributes": "Password"
+}</t>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -718,7 +725,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{FACCEB44-97B3-401B-BD48-08626DAD862C}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1001,15 +1008,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="28.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="1"/>
+    <col min="1" max="1" width="8.58203125" style="1"/>
+    <col min="2" max="2" width="15.58203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="28.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.58203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1035,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="131.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="126">
       <c r="A3" s="9" t="s">
         <v>100</v>
       </c>
@@ -1079,7 +1086,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="187.5">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="180">
       <c r="A4" s="9" t="s">
         <v>47</v>
       </c>
@@ -1100,7 +1107,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A5" s="9" t="s">
         <v>47</v>
       </c>
@@ -1121,49 +1128,49 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="168.75">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="162">
       <c r="A6" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="131.25">
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A7" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="93.75">
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
@@ -1184,7 +1191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="144">
       <c r="A9" s="9" t="s">
         <v>47</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="150">
+    <row r="10" spans="1:7" ht="144">
       <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
@@ -1226,7 +1233,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="168.75">
+    <row r="11" spans="1:7" ht="162">
       <c r="A11" s="9" t="s">
         <v>47</v>
       </c>
@@ -1249,7 +1256,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="93.75">
+    <row r="12" spans="1:7" ht="90">
       <c r="A12" s="9" t="s">
         <v>47</v>
       </c>
@@ -1270,7 +1277,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="93.75">
+    <row r="13" spans="1:7" ht="90">
       <c r="A13" s="9" t="s">
         <v>47</v>
       </c>
@@ -1291,7 +1298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75">
+    <row r="14" spans="1:7" ht="72">
       <c r="A14" s="9" t="s">
         <v>47</v>
       </c>
@@ -1312,7 +1319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="168.75">
+    <row r="15" spans="1:7" ht="162">
       <c r="A15" s="9" t="s">
         <v>47</v>
       </c>
@@ -1335,7 +1342,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="150">
+    <row r="16" spans="1:7" ht="144">
       <c r="A16" s="9" t="s">
         <v>47</v>
       </c>
@@ -1356,7 +1363,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="112.5">
+    <row r="17" spans="1:7" ht="126">
       <c r="A17" s="9" t="s">
         <v>105</v>
       </c>
@@ -1366,18 +1373,20 @@
       <c r="C17" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="E17" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.75">
+    </row>
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="90">
       <c r="A18" s="9" t="s">
         <v>100</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="131.25">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="126">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="112.5">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="108">
       <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
@@ -1442,7 +1451,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="150">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="144">
       <c r="A21" s="9" t="s">
         <v>47</v>
       </c>
@@ -1465,7 +1474,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="75">
+    <row r="22" spans="1:7" ht="54">
       <c r="A22" s="9" t="s">
         <v>47</v>
       </c>
@@ -1473,7 +1482,7 @@
         <v>50</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="6" t="s">
@@ -1486,7 +1495,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75">
+    <row r="23" spans="1:7" ht="72">
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
@@ -1494,7 +1503,7 @@
         <v>53</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
@@ -1507,7 +1516,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="93.75">
+    <row r="24" spans="1:7" ht="90">
       <c r="A24" s="9" t="s">
         <v>47</v>
       </c>
@@ -1515,40 +1524,40 @@
         <v>48</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="6" t="s">
         <v>56</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="12" customFormat="1" ht="75">
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="72">
       <c r="A25" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F25" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1578,14 +1587,14 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="5" width="28.375" customWidth="1"/>
-    <col min="6" max="6" width="49.875" customWidth="1"/>
-    <col min="7" max="7" width="40.125" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="49.83203125" customWidth="1"/>
+    <col min="7" max="7" width="40.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1611,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
       <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
@@ -1632,7 +1641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="56.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="54">
       <c r="A3" s="9" t="s">
         <v>47</v>
       </c>
@@ -1653,27 +1662,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="262.5">
+    <row r="4" spans="1:7" ht="252">
       <c r="A4" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update regular expressions used in check arguments
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5423F2D1-8B6C-492E-A42B-3EA2CD9A37EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6B7504-62A1-4DF2-BD1F-5530C9FE0397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -413,18 +413,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>{ 
-"NamingPattern" : "(^(dt_)*([A-Z][a-z0-9]*)+$)"
-}</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>{ 
-"NamingPattern" : "(^(in_|out_|io_)(dt_)*([A-Z][a-z0-9]*)+)"
-}</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>Arguments</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -550,6 +538,16 @@
     <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.
 Limitation: It can give false alerts for variables binded to InOut argumets inside repetitive structures.</t>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>{ 
+"NamingPattern" : "(^(dt_)?([A-Z][a-z0-9]*)+$)"
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"NamingPattern" : "(^(in_|out_|io_)(dt_)?([A-Z][a-z0-9]*)+)"
+}</t>
   </si>
 </sst>
 </file>
@@ -560,14 +558,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -575,7 +573,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -583,7 +581,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -591,28 +589,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -999,17 +997,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="28.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="1"/>
+    <col min="1" max="1" width="8.6328125" style="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="28.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1023,7 +1023,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="116">
       <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>45</v>
@@ -1058,15 +1058,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="131.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="101.5">
       <c r="A3" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -1079,7 +1079,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="187.5">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="145">
       <c r="A4" s="9" t="s">
         <v>47</v>
       </c>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>31</v>
@@ -1100,7 +1100,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A5" s="9" t="s">
         <v>47</v>
       </c>
@@ -1121,49 +1121,49 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="168.75">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="130.5">
       <c r="A6" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="72.5">
+      <c r="A7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="131.25">
-      <c r="A7" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="93.75">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="116">
       <c r="A9" s="9" t="s">
         <v>47</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>38</v>
@@ -1205,7 +1205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="150">
+    <row r="10" spans="1:7" ht="116">
       <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>37</v>
@@ -1226,7 +1226,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="168.75">
+    <row r="11" spans="1:7" ht="130.5">
       <c r="A11" s="9" t="s">
         <v>47</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>93</v>
@@ -1249,7 +1249,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="93.75">
+    <row r="12" spans="1:7" ht="72.5">
       <c r="A12" s="9" t="s">
         <v>47</v>
       </c>
@@ -1264,13 +1264,13 @@
         <v>56</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="93.75">
+    <row r="13" spans="1:7" ht="72.5">
       <c r="A13" s="9" t="s">
         <v>47</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75">
+    <row r="14" spans="1:7" ht="58">
       <c r="A14" s="9" t="s">
         <v>47</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="168.75">
+    <row r="15" spans="1:7" ht="130.5">
       <c r="A15" s="9" t="s">
         <v>47</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>22</v>
@@ -1335,7 +1335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="150">
+    <row r="16" spans="1:7" ht="116">
       <c r="A16" s="9" t="s">
         <v>47</v>
       </c>
@@ -1350,36 +1350,36 @@
         <v>56</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="112.5">
+    <row r="17" spans="1:7" ht="87">
       <c r="A17" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.75">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="72.5">
       <c r="A18" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>71</v>
@@ -1398,7 +1398,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="131.25">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="101.5">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="112.5">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="87">
       <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="150">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="116">
       <c r="A21" s="9" t="s">
         <v>47</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>81</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>45</v>
@@ -1465,7 +1465,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="75">
+    <row r="22" spans="1:7" ht="43.5">
       <c r="A22" s="9" t="s">
         <v>47</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>50</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="6" t="s">
@@ -1486,7 +1486,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75">
+    <row r="23" spans="1:7" ht="58">
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>53</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
@@ -1507,7 +1507,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="93.75">
+    <row r="24" spans="1:7" ht="72.5">
       <c r="A24" s="9" t="s">
         <v>47</v>
       </c>
@@ -1515,40 +1515,40 @@
         <v>48</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="6" t="s">
         <v>56</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="12" customFormat="1" ht="75">
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="58">
       <c r="A25" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1578,14 +1578,14 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="5" width="28.375" customWidth="1"/>
-    <col min="6" max="6" width="49.875" customWidth="1"/>
-    <col min="7" max="7" width="40.125" customWidth="1"/>
+    <col min="1" max="1" width="8.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.90625" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" customWidth="1"/>
+    <col min="4" max="5" width="28.36328125" customWidth="1"/>
+    <col min="6" max="6" width="49.90625" customWidth="1"/>
+    <col min="7" max="7" width="40.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1611,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="56.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="43.5">
       <c r="A3" s="9" t="s">
         <v>47</v>
       </c>
@@ -1653,27 +1653,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="262.5">
+    <row r="4" spans="1:7" ht="203">
       <c r="A4" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add UnadjustedForEach check and change folder name from JP to JA
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958EAFE8-C9D9-4D1E-BB20-EE9D912644E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A5CFDF-360A-4289-B742-BBF278A12401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="146">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -553,12 +553,6 @@
 } </t>
   </si>
   <si>
-    <t>Workflows should contain only activities allowed by the Centre of Excellence (COE). If an activity is present in the blacklist or is not present in the whitelist, it should not be used. The whitelist and the blacklist are passed as arguments to this check, and they contain names of activities as specified by the last part of their class name (for example, "Sequence" instead of "System.Activities.Statements.Sequence" and "SetCredential" instead of "UiPath.Core.Activities.SetCredential"). The class name of an activity can be found at the top of the Properties panel in UiPath Studio.</t>
-  </si>
-  <si>
-    <t>Remove the activity or request its addition to the activities whitelist (or its removal from the activities blacklist).</t>
-  </si>
-  <si>
     <t>Yes</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -577,6 +571,27 @@
   </si>
   <si>
     <t>Add a Log Message activity immediately before or immediately after Open Browser and log the URL used in the Open Browser activity.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Unadjusted For Each</t>
+  </si>
+  <si>
+    <t>Checks\Standard\UnadjustedForEach.xaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify the type and the name of the "item" loop variable in the For Each activity to match the data being processed. </t>
+  </si>
+  <si>
+    <t>To further improve the readability of the workflow, it is recommended to change the name and type of the "item" loop variable in the For Each activity according to the data being processed.</t>
+  </si>
+  <si>
+    <t>Workflows should contain only activities allowed by the Centre of Excellence (CoE). If an activity is present in the blacklist or is not present in the whitelist of activities, it should not be used. The whitelist and the blacklist are passed as arguments to this check and contain the names of the unallowed activities. Each name must be specified in the the same way as the last part of the activity's class name (for example, "Sequence" instead of "System.Activities.Statements.Sequence" and "SetCredential" instead of "UiPath.Core.Activities.SetCredential"). The class name of an activity can be found at the top of the Properties panel in UiPath Studio.</t>
+  </si>
+  <si>
+    <t>Remove the activity from the workflow or request its addition to the activities whitelist (or its removal from the activities blacklist).</t>
   </si>
 </sst>
 </file>
@@ -587,14 +602,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -602,7 +617,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -610,7 +625,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -618,28 +633,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1024,19 +1039,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="15.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="28.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="1"/>
+    <col min="1" max="1" width="8.6328125" style="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="28.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.6328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1062,9 +1079,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="116">
       <c r="A2" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>16</v>
@@ -1085,9 +1102,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="131.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="101.5">
       <c r="A3" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>59</v>
@@ -1106,9 +1123,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="187.5">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="145">
       <c r="A4" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>32</v>
@@ -1127,9 +1144,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A5" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>42</v>
@@ -1148,9 +1165,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="168.75">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="130.5">
       <c r="A6" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>112</v>
@@ -1169,9 +1186,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="131.25">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A7" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>116</v>
@@ -1190,9 +1207,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A8" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>11</v>
@@ -1211,9 +1228,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="150">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="116">
       <c r="A9" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>40</v>
@@ -1232,9 +1249,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="150">
+    <row r="10" spans="1:7" ht="116">
       <c r="A10" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>41</v>
@@ -1253,9 +1270,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="168.75">
+    <row r="11" spans="1:7" ht="130.5">
       <c r="A11" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>72</v>
@@ -1276,9 +1293,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="93.75">
+    <row r="12" spans="1:7" ht="72.5">
       <c r="A12" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>62</v>
@@ -1297,9 +1314,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="93.75">
+    <row r="13" spans="1:7" ht="72.5">
       <c r="A13" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>5</v>
@@ -1318,9 +1335,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75">
+    <row r="14" spans="1:7" ht="58">
       <c r="A14" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
@@ -1339,9 +1356,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="168.75">
+    <row r="15" spans="1:7" ht="130.5">
       <c r="A15" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>24</v>
@@ -1362,9 +1379,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="150">
+    <row r="16" spans="1:7" ht="116">
       <c r="A16" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>64</v>
@@ -1383,9 +1400,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="112.5">
+    <row r="17" spans="1:7" ht="87">
       <c r="A17" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>103</v>
@@ -1404,9 +1421,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.75">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="72.5">
       <c r="A18" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>70</v>
@@ -1425,9 +1442,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="131.25">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="101.5">
       <c r="A19" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>14</v>
@@ -1446,9 +1463,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="112.5">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="87">
       <c r="A20" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>56</v>
@@ -1469,9 +1486,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="150">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="116">
       <c r="A21" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>19</v>
@@ -1492,9 +1509,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="75">
+    <row r="22" spans="1:7" ht="43.5">
       <c r="A22" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>49</v>
@@ -1513,9 +1530,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75">
+    <row r="23" spans="1:7" ht="58">
       <c r="A23" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>52</v>
@@ -1534,9 +1551,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="93.75">
+    <row r="24" spans="1:7" ht="72.5">
       <c r="A24" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>47</v>
@@ -1555,70 +1572,91 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="225">
+    <row r="25" spans="1:7" ht="58">
       <c r="A25" s="9" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>132</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D25" s="9"/>
       <c r="E25" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="75">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="188.5">
       <c r="A26" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="9"/>
+        <v>131</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="E26" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="12" customFormat="1" ht="75">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="58">
       <c r="A27" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="12" customFormat="1" ht="58">
+      <c r="A28" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D28" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="9" t="s">
+      <c r="E28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1628,13 +1666,13 @@
   </sortState>
   <phoneticPr fontId="6"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E27" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E28" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E10" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
       <formula1>"Fix, Double-check"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A27" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A28" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1649,14 +1687,14 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="5" width="28.375" customWidth="1"/>
-    <col min="6" max="6" width="49.875" customWidth="1"/>
-    <col min="7" max="7" width="40.125" customWidth="1"/>
+    <col min="1" max="1" width="8.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.90625" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" customWidth="1"/>
+    <col min="4" max="5" width="28.36328125" customWidth="1"/>
+    <col min="6" max="6" width="49.90625" customWidth="1"/>
+    <col min="7" max="7" width="40.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1682,9 +1720,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="93.75">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A2" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>30</v>
@@ -1703,9 +1741,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="56.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="43.5">
       <c r="A3" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>71</v>
@@ -1724,7 +1762,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="262.5">
+    <row r="4" spans="1:7" ht="203">
       <c r="A4" s="9" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
Add Unallowed Application check
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA54756-89E6-4344-A86E-B18BB3C72A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDAF018-2C55-4816-AFD7-538A2A836896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="155">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -604,6 +604,24 @@
   </si>
   <si>
     <t>Make sure the project contains the entry point workflow as defined in project.json.</t>
+  </si>
+  <si>
+    <t>Unallowed application</t>
+  </si>
+  <si>
+    <t>Checks\Custom\UnallowedApplication.xaml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+"WhiteList" : "",
+"BlackList": "notepad.exe,explorer.exe"
+} </t>
+  </si>
+  <si>
+    <t>Remove interactions with unallowed applications from the workflow or request the addition of the application to the whitelist (or its removal from the blacklist).</t>
+  </si>
+  <si>
+    <t>Workflows should interact only with applications allowed by the Centre of Excellence (CoE). If an application is present in the blacklist or is not present in the whitelist of activities, it should not be used by the robot. The whitelist and the blacklist are passed as arguments to this check and contain names of applications' executable files. Each name must be specified as the application's executable file name (for example, "notepad.exe" instead of "Notepad").</t>
   </si>
 </sst>
 </file>
@@ -1054,7 +1072,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1631,47 +1649,70 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="58">
+    <row r="27" spans="1:7" ht="130.5">
       <c r="A27" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D27" s="9"/>
+        <v>151</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>152</v>
+      </c>
       <c r="E27" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="12" customFormat="1" ht="58">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="58">
       <c r="A28" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="12" customFormat="1" ht="58">
+      <c r="A29" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="9" t="s">
+      <c r="E29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1681,13 +1722,13 @@
   </sortState>
   <phoneticPr fontId="6"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E28" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E29" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E10" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
       <formula1>"Fix, Double-check"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A28" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A29" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update regular expressions of naming conventions
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BFACE4-C8A7-486A-AB69-6A330A22F9E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636FD782-3A9E-4B2D-8B67-F29F73DC242C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,18 +417,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>{ 
-"NamingPattern" : "(^(dt_)*([A-Z][a-z0-9]*)+$)"
-}</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>{ 
-"NamingPattern" : "(^(in_|out_|io_)(dt_)*([A-Z][a-z0-9]*)+)"
-}</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>Arguments</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -617,12 +605,6 @@
     <t>Checks\Custom\UnallowedApplication.xaml</t>
   </si>
   <si>
-    <t xml:space="preserve">{
-"WhiteList" : "",
-"BlackList": "notepad.exe,explorer.exe"
-} </t>
-  </si>
-  <si>
     <t>Remove interactions with unallowed applications from the workflow or request the addition of the application to the whitelist (or its removal from the blacklist).</t>
   </si>
   <si>
@@ -660,6 +642,22 @@
   </si>
   <si>
     <t>If the process is to be run on Unattended robots, remove activities that expect user interaction.</t>
+  </si>
+  <si>
+    <t>{ 
+"NamingPattern" : "(^(dt_)?([A-Z][a-z0-9]*)+$)"
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"NamingPattern" : "(^(in_|out_|io_)(dt_)?([A-Z][a-z0-9]*)+)"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+"WhiteList" : "",
+"BlackList": "application1.exe,application2.exe"
+} </t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1136,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>44</v>
@@ -1152,7 +1150,7 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="116">
       <c r="A2" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>16</v>
@@ -1161,7 +1159,7 @@
         <v>79</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>45</v>
@@ -1175,13 +1173,13 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="101.5">
       <c r="A3" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
@@ -1196,7 +1194,7 @@
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="145">
       <c r="A4" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>32</v>
@@ -1206,7 +1204,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>31</v>
@@ -1217,7 +1215,7 @@
     </row>
     <row r="5" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A5" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>42</v>
@@ -1238,49 +1236,49 @@
     </row>
     <row r="6" spans="1:7" s="5" customFormat="1" ht="130.5">
       <c r="A6" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A7" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A8" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>11</v>
@@ -1301,7 +1299,7 @@
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" ht="116">
       <c r="A9" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>40</v>
@@ -1311,7 +1309,7 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>38</v>
@@ -1322,7 +1320,7 @@
     </row>
     <row r="10" spans="1:7" ht="116">
       <c r="A10" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>41</v>
@@ -1332,7 +1330,7 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>37</v>
@@ -1343,13 +1341,13 @@
     </row>
     <row r="11" spans="1:7" ht="130.5">
       <c r="A11" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>92</v>
@@ -1366,7 +1364,7 @@
     </row>
     <row r="12" spans="1:7" ht="72.5">
       <c r="A12" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>62</v>
@@ -1379,7 +1377,7 @@
         <v>55</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>63</v>
@@ -1387,7 +1385,7 @@
     </row>
     <row r="13" spans="1:7" ht="72.5">
       <c r="A13" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>5</v>
@@ -1408,7 +1406,7 @@
     </row>
     <row r="14" spans="1:7" ht="58">
       <c r="A14" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
@@ -1429,7 +1427,7 @@
     </row>
     <row r="15" spans="1:7" ht="130.5">
       <c r="A15" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>24</v>
@@ -1441,7 +1439,7 @@
         <v>94</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>22</v>
@@ -1452,7 +1450,7 @@
     </row>
     <row r="16" spans="1:7" ht="116">
       <c r="A16" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>64</v>
@@ -1465,7 +1463,7 @@
         <v>55</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>65</v>
@@ -1473,28 +1471,28 @@
     </row>
     <row r="17" spans="1:7" ht="87">
       <c r="A17" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="12" customFormat="1" ht="72.5">
       <c r="A18" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>70</v>
@@ -1515,7 +1513,7 @@
     </row>
     <row r="19" spans="1:7" s="12" customFormat="1" ht="101.5">
       <c r="A19" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>14</v>
@@ -1536,7 +1534,7 @@
     </row>
     <row r="20" spans="1:7" s="12" customFormat="1" ht="87">
       <c r="A20" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>56</v>
@@ -1559,7 +1557,7 @@
     </row>
     <row r="21" spans="1:7" s="12" customFormat="1" ht="116">
       <c r="A21" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>19</v>
@@ -1568,7 +1566,7 @@
         <v>80</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>45</v>
@@ -1582,13 +1580,13 @@
     </row>
     <row r="22" spans="1:7" ht="43.5">
       <c r="A22" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="6" t="s">
@@ -1603,13 +1601,13 @@
     </row>
     <row r="23" spans="1:7" ht="58">
       <c r="A23" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
@@ -1624,20 +1622,20 @@
     </row>
     <row r="24" spans="1:7" ht="72.5">
       <c r="A24" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>48</v>
@@ -1645,157 +1643,157 @@
     </row>
     <row r="25" spans="1:7" ht="58">
       <c r="A25" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="188.5">
       <c r="A26" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>131</v>
-      </c>
       <c r="E26" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="130.5">
       <c r="A27" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="58">
       <c r="A28" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="12" customFormat="1" ht="58">
       <c r="A29" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="E29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G29" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="12" customFormat="1" ht="72.5">
       <c r="A30" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B30" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="12" customFormat="1" ht="101.5">
       <c r="A31" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1862,7 +1860,7 @@
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="72.5">
       <c r="A2" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>30</v>
@@ -1883,7 +1881,7 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="43.5">
       <c r="A3" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>71</v>
@@ -1904,46 +1902,46 @@
     </row>
     <row r="4" spans="1:7" s="5" customFormat="1" ht="58">
       <c r="A4" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="203">
       <c r="A5" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="E5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Unsuitable Exception Type check
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636FD782-3A9E-4B2D-8B67-F29F73DC242C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75F8D3E-A220-4AF4-928D-B93F763873B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="168">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -658,6 +658,18 @@
 "WhiteList" : "",
 "BlackList": "application1.exe,application2.exe"
 } </t>
+  </si>
+  <si>
+    <t>Checks\Custom\UnsuitableExceptionType.xaml</t>
+  </si>
+  <si>
+    <t>Unsuitable exception type</t>
+  </si>
+  <si>
+    <t>When throwing exceptions, it is recommended to properly distinguish between application-originated and business-originated exceptions. The type of the exception to be thrown or caught should be as specific as possible, and Exception and ApplicationException should be avoided.</t>
+  </si>
+  <si>
+    <t>Use specific exception types and avoid using generic types such as Exception and ApplicationException.</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1120,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1796,19 +1808,40 @@
         <v>160</v>
       </c>
     </row>
+    <row r="32" spans="1:7" s="12" customFormat="1" ht="87">
+      <c r="A32" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G24">
     <sortCondition descending="1" ref="C2:C24"/>
   </sortState>
   <phoneticPr fontId="6"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E31" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E32" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E10" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
       <formula1>"Fix, Double-check"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A31" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A32" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Included Read Only Property Of Constant check
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75F8D3E-A220-4AF4-928D-B93F763873B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5ED2C4-1ECE-4978-812B-9C97383C2068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="173">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -670,6 +670,24 @@
   </si>
   <si>
     <t>Use specific exception types and avoid using generic types such as Exception and ApplicationException.</t>
+  </si>
+  <si>
+    <t>Checks\Custom\ReadOnlyPropertyOfConstant.xaml</t>
+  </si>
+  <si>
+    <t>ReadOnly property of constant</t>
+  </si>
+  <si>
+    <t>{ 
+"NamingPattern" : "(^([A-Z][A-Z0-9]*)$)"
+}</t>
+  </si>
+  <si>
+    <t>Constant is a variable that does not change the value set by the default value. 
+It must follow a specific naming convention so that it can be distinguished from other variables. In addition, ReadOnly must be specified in the variable's Modifiers property.</t>
+  </si>
+  <si>
+    <t>Variables that do not have their values modified should follow the naming convention of constants and have ReadOnly checked in their Modifiers property.</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1138,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1829,19 +1847,42 @@
         <v>167</v>
       </c>
     </row>
+    <row r="33" spans="1:7" s="12" customFormat="1" ht="87">
+      <c r="A33" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G24">
     <sortCondition descending="1" ref="C2:C24"/>
   </sortState>
   <phoneticPr fontId="6"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E32" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E33" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E10" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
       <formula1>"Fix, Double-check"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A32" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A33" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Include Directly Send Outlook Mail check
</commit_message>
<xml_diff>
--- a/Config/EN/Checklist.xlsx
+++ b/Config/EN/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5ED2C4-1ECE-4978-812B-9C97383C2068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAE6F48-37BB-4B16-A3E2-1A208EE73A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="177">
   <si>
     <t>Explanation</t>
     <phoneticPr fontId="6"/>
@@ -688,6 +688,18 @@
   </si>
   <si>
     <t>Variables that do not have their values modified should follow the naming convention of constants and have ReadOnly checked in their Modifiers property.</t>
+  </si>
+  <si>
+    <t>Directly send Outlook mail</t>
+  </si>
+  <si>
+    <t>Checks\Custom\DirectlySendOutlookMail.xaml</t>
+  </si>
+  <si>
+    <t>According to the CoE (Centre of Excellence)'s security policies, robots should not be allowed to directly send emails. Instead, emails created by robots should be saved as drafts and then reviewed by humans before sending.</t>
+  </si>
+  <si>
+    <t>Check the IsDraft property of Send Outlook Mail Message activities, as specified by the CoE's security policies.</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1150,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1870,19 +1882,40 @@
         <v>172</v>
       </c>
     </row>
+    <row r="34" spans="1:7" s="12" customFormat="1" ht="58">
+      <c r="A34" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G24">
     <sortCondition descending="1" ref="C2:C24"/>
   </sortState>
   <phoneticPr fontId="6"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E33" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11:E34" xr:uid="{0C119EAA-8F59-4C40-BAC5-92844DA1C56B}">
       <formula1>"Fix, Double check"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E10" xr:uid="{2638BF1E-DAA8-4285-8C2C-D6CD2C75FF08}">
       <formula1>"Fix, Double-check"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A33" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A34" xr:uid="{A34D1090-DD85-4AC6-BEEC-A12FA4A5B391}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>